<commit_message>
run new version 5
</commit_message>
<xml_diff>
--- a/All_datasets.xlsx
+++ b/All_datasets.xlsx
@@ -5303,7 +5303,7 @@
         <v>1.01955413479884</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002727262931784652</v>
+        <v>0.003272830709032061</v>
       </c>
       <c r="D2" t="n">
         <v>-0.09468368881641709</v>
@@ -5318,7 +5318,7 @@
         <v>2.739</v>
       </c>
       <c r="H2" t="n">
-        <v>0.000547878</v>
+        <v>0.004891327390165</v>
       </c>
       <c r="I2" t="n">
         <v>-0.09468368881641709</v>
@@ -5337,7 +5337,7 @@
         <v>1.019261501905951</v>
       </c>
       <c r="C3" t="n">
-        <v>0.004366399591716795</v>
+        <v>0.005650426376028693</v>
       </c>
       <c r="D3" t="n">
         <v>-0.09461263669183584</v>
@@ -5352,7 +5352,7 @@
         <v>2.749</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0005497190000000001</v>
+        <v>0.009688163830732999</v>
       </c>
       <c r="I3" t="n">
         <v>-0.09461263669183584</v>
@@ -5371,7 +5371,7 @@
         <v>1.019092986583491</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003428262062275564</v>
+        <v>0.004607684167324609</v>
       </c>
       <c r="D4" t="n">
         <v>-0.09493052876059216</v>
@@ -5386,7 +5386,7 @@
         <v>2.756</v>
       </c>
       <c r="H4" t="n">
-        <v>0.000551123</v>
+        <v>0.008343878597812</v>
       </c>
       <c r="I4" t="n">
         <v>-0.09493052876059216</v>
@@ -5405,7 +5405,7 @@
         <v>1.01920468111376</v>
       </c>
       <c r="C5" t="n">
-        <v>0.002474593453094589</v>
+        <v>0.003023750828807779</v>
       </c>
       <c r="D5" t="n">
         <v>-0.09460199638093547</v>
@@ -5420,7 +5420,7 @@
         <v>2.756</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000551259</v>
+        <v>0.004730974720984</v>
       </c>
       <c r="I5" t="n">
         <v>-0.09460199638093547</v>
@@ -5439,7 +5439,7 @@
         <v>1.019102067054115</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003085895778865776</v>
+        <v>0.003853908176653013</v>
       </c>
       <c r="D6" t="n">
         <v>-0.09461164680031775</v>
@@ -5454,7 +5454,7 @@
         <v>2.749</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000549895</v>
+        <v>0.006251745842114</v>
       </c>
       <c r="I6" t="n">
         <v>-0.09461164680031775</v>
@@ -5473,7 +5473,7 @@
         <v>1.019098138575958</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00323301063452513</v>
+        <v>0.004030123570657592</v>
       </c>
       <c r="D7" t="n">
         <v>-0.0947113851968906</v>
@@ -5488,7 +5488,7 @@
         <v>2.752</v>
       </c>
       <c r="H7" t="n">
-        <v>0.000550481</v>
+        <v>0.006520897917793</v>
       </c>
       <c r="I7" t="n">
         <v>-0.0947113851968906</v>
@@ -5507,7 +5507,7 @@
         <v>1.019075735219341</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002909525172730187</v>
+        <v>0.003756982541617064</v>
       </c>
       <c r="D8" t="n">
         <v>-0.09498309447476005</v>
@@ -5522,7 +5522,7 @@
         <v>2.753</v>
       </c>
       <c r="H8" t="n">
-        <v>0.000550533</v>
+        <v>0.006444634638151</v>
       </c>
       <c r="I8" t="n">
         <v>-0.09498309447476005</v>
@@ -5541,7 +5541,7 @@
         <v>1.018841099849396</v>
       </c>
       <c r="C9" t="n">
-        <v>0.003402162084148781</v>
+        <v>0.00495261354136049</v>
       </c>
       <c r="D9" t="n">
         <v>-0.09458392019252382</v>
@@ -5556,7 +5556,7 @@
         <v>2.746</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00054919</v>
+        <v>0.009715954243424</v>
       </c>
       <c r="I9" t="n">
         <v>-0.09458392019252382</v>
@@ -5575,7 +5575,7 @@
         <v>1.019176444798685</v>
       </c>
       <c r="C10" t="n">
-        <v>0.002894534635686457</v>
+        <v>0.00400428446379558</v>
       </c>
       <c r="D10" t="n">
         <v>-0.09456147092396305</v>
@@ -5590,7 +5590,7 @@
         <v>2.76</v>
       </c>
       <c r="H10" t="n">
-        <v>0.000551925</v>
+        <v>0.007513366549737</v>
       </c>
       <c r="I10" t="n">
         <v>-0.09456147092396305</v>
@@ -5609,7 +5609,7 @@
         <v>1.019313135262444</v>
       </c>
       <c r="C11" t="n">
-        <v>0.005397927985709474</v>
+        <v>0.007295502197423162</v>
       </c>
       <c r="D11" t="n">
         <v>-0.09471901459374377</v>
@@ -5624,7 +5624,7 @@
         <v>2.751</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00055021</v>
+        <v>0.013257029325526</v>
       </c>
       <c r="I11" t="n">
         <v>-0.09471901459374377</v>
@@ -5643,7 +5643,7 @@
         <v>1.018037974265213</v>
       </c>
       <c r="C12" t="n">
-        <v>0.004021363958810756</v>
+        <v>0.005151192163864313</v>
       </c>
       <c r="D12" t="n">
         <v>-0.1186007078629865</v>
@@ -5658,7 +5658,7 @@
         <v>2.761</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0005521499999999999</v>
+        <v>0.008748237670929001</v>
       </c>
       <c r="I12" t="n">
         <v>-0.1186007078629865</v>
@@ -5677,7 +5677,7 @@
         <v>1.018413370767813</v>
       </c>
       <c r="C13" t="n">
-        <v>0.003801090636467539</v>
+        <v>0.005501334526828454</v>
       </c>
       <c r="D13" t="n">
         <v>-0.1188698326590361</v>
@@ -5692,7 +5692,7 @@
         <v>2.757</v>
       </c>
       <c r="H13" t="n">
-        <v>0.000551371</v>
+        <v>0.010780406878195</v>
       </c>
       <c r="I13" t="n">
         <v>-0.1188698326590361</v>
@@ -5711,7 +5711,7 @@
         <v>1.018343700268765</v>
       </c>
       <c r="C14" t="n">
-        <v>0.003964453143655546</v>
+        <v>0.005371576867214532</v>
       </c>
       <c r="D14" t="n">
         <v>-0.1186059136544484</v>
@@ -5726,7 +5726,7 @@
         <v>2.761</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0005521429999999999</v>
+        <v>0.009842461528008</v>
       </c>
       <c r="I14" t="n">
         <v>-0.1186059136544484</v>
@@ -5745,7 +5745,7 @@
         <v>1.018477952815318</v>
       </c>
       <c r="C15" t="n">
-        <v>0.002635570880354945</v>
+        <v>0.00307827730646071</v>
       </c>
       <c r="D15" t="n">
         <v>-0.1180289245665194</v>
@@ -5760,7 +5760,7 @@
         <v>2.757</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00055136</v>
+        <v>0.004340500589592</v>
       </c>
       <c r="I15" t="n">
         <v>-0.1180289245665194</v>
@@ -5779,7 +5779,7 @@
         <v>1.018494187448801</v>
       </c>
       <c r="C16" t="n">
-        <v>0.00530984915594112</v>
+        <v>0.00776566628364966</v>
       </c>
       <c r="D16" t="n">
         <v>-0.1190525439858523</v>
@@ -5794,7 +5794,7 @@
         <v>2.761</v>
       </c>
       <c r="H16" t="n">
-        <v>0.000552117</v>
+        <v>0.015371477021473</v>
       </c>
       <c r="I16" t="n">
         <v>-0.1190525439858523</v>
@@ -5813,7 +5813,7 @@
         <v>1.019093297623116</v>
       </c>
       <c r="C17" t="n">
-        <v>0.003008083837759189</v>
+        <v>0.004047479819917342</v>
       </c>
       <c r="D17" t="n">
         <v>-0.1188203516166466</v>
@@ -5828,7 +5828,7 @@
         <v>2.744</v>
       </c>
       <c r="H17" t="n">
-        <v>0.000548816</v>
+        <v>0.007312286604905</v>
       </c>
       <c r="I17" t="n">
         <v>-0.1188203516166466</v>
@@ -5847,7 +5847,7 @@
         <v>1.01815527775581</v>
       </c>
       <c r="C18" t="n">
-        <v>0.005084010327959773</v>
+        <v>0.007561857254133796</v>
       </c>
       <c r="D18" t="n">
         <v>-0.1187594703689183</v>
@@ -5862,7 +5862,7 @@
         <v>2.753</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0005506140000000001</v>
+        <v>0.015145754960434</v>
       </c>
       <c r="I18" t="n">
         <v>-0.1187594703689183</v>
@@ -5881,7 +5881,7 @@
         <v>1.017900904988349</v>
       </c>
       <c r="C19" t="n">
-        <v>0.004888293682926267</v>
+        <v>0.007370482014416724</v>
       </c>
       <c r="D19" t="n">
         <v>-0.118398307234427</v>
@@ -5896,7 +5896,7 @@
         <v>2.757</v>
       </c>
       <c r="H19" t="n">
-        <v>0.000551356</v>
+        <v>0.014950912307602</v>
       </c>
       <c r="I19" t="n">
         <v>-0.118398307234427</v>
@@ -5915,7 +5915,7 @@
         <v>1.018783375294373</v>
       </c>
       <c r="C20" t="n">
-        <v>0.003923529700670683</v>
+        <v>0.005224319725925793</v>
       </c>
       <c r="D20" t="n">
         <v>-0.1195153545433347</v>
@@ -5930,7 +5930,7 @@
         <v>2.753</v>
       </c>
       <c r="H20" t="n">
-        <v>0.000550681</v>
+        <v>0.009337787552397</v>
       </c>
       <c r="I20" t="n">
         <v>-0.1195153545433347</v>
@@ -5949,7 +5949,7 @@
         <v>1.018516313126167</v>
       </c>
       <c r="C21" t="n">
-        <v>0.002900375987305232</v>
+        <v>0.003793783654166793</v>
       </c>
       <c r="D21" t="n">
         <v>-0.1184922992798134</v>
@@ -5964,7 +5964,7 @@
         <v>2.755</v>
       </c>
       <c r="H21" t="n">
-        <v>0.000550957</v>
+        <v>0.006637853615773</v>
       </c>
       <c r="I21" t="n">
         <v>-0.1184922992798134</v>
@@ -5983,7 +5983,7 @@
         <v>1.01843940537399</v>
       </c>
       <c r="C22" t="n">
-        <v>0.003800065894958993</v>
+        <v>0.005217645819351358</v>
       </c>
       <c r="D22" t="n">
         <v>-0.1519605918834235</v>
@@ -5998,7 +5998,7 @@
         <v>5.578</v>
       </c>
       <c r="H22" t="n">
-        <v>0.001115628</v>
+        <v>0.019614124125092</v>
       </c>
       <c r="I22" t="n">
         <v>-0.1519605918834235</v>
@@ -6017,7 +6017,7 @@
         <v>1.017730243177382</v>
       </c>
       <c r="C23" t="n">
-        <v>0.001940541796348569</v>
+        <v>0.002862661943250054</v>
       </c>
       <c r="D23" t="n">
         <v>-0.1516432644978034</v>
@@ -6032,7 +6032,7 @@
         <v>5.573</v>
       </c>
       <c r="H23" t="n">
-        <v>0.001114562</v>
+        <v>0.011578099655723</v>
       </c>
       <c r="I23" t="n">
         <v>-0.1516432644978034</v>
@@ -6051,7 +6051,7 @@
         <v>1.017711034216828</v>
       </c>
       <c r="C24" t="n">
-        <v>0.004539838697563177</v>
+        <v>0.006137682113597089</v>
       </c>
       <c r="D24" t="n">
         <v>-0.1521381790959864</v>
@@ -6066,7 +6066,7 @@
         <v>5.582</v>
       </c>
       <c r="H24" t="n">
-        <v>0.001116311</v>
+        <v>0.022682673887978</v>
       </c>
       <c r="I24" t="n">
         <v>-0.1521381790959864</v>
@@ -6085,7 +6085,7 @@
         <v>1.018575221931231</v>
       </c>
       <c r="C25" t="n">
-        <v>0.003890918079105336</v>
+        <v>0.005213595663293753</v>
       </c>
       <c r="D25" t="n">
         <v>-0.1523009152981192</v>
@@ -6100,7 +6100,7 @@
         <v>5.567</v>
       </c>
       <c r="H25" t="n">
-        <v>0.001113371</v>
+        <v>0.018998988836365</v>
       </c>
       <c r="I25" t="n">
         <v>-0.1523009152981192</v>
@@ -6119,7 +6119,7 @@
         <v>1.017924185605009</v>
       </c>
       <c r="C26" t="n">
-        <v>0.002287883311508676</v>
+        <v>0.003147999350854616</v>
       </c>
       <c r="D26" t="n">
         <v>-0.1518716401407625</v>
@@ -6134,7 +6134,7 @@
         <v>5.578</v>
       </c>
       <c r="H26" t="n">
-        <v>0.001115576</v>
+        <v>0.011901262011855</v>
       </c>
       <c r="I26" t="n">
         <v>-0.1518716401407625</v>
@@ -6153,7 +6153,7 @@
         <v>1.018381879256725</v>
       </c>
       <c r="C27" t="n">
-        <v>0.005223860833804657</v>
+        <v>0.00755499268938638</v>
       </c>
       <c r="D27" t="n">
         <v>-0.1523297439645124</v>
@@ -6168,7 +6168,7 @@
         <v>5.546</v>
       </c>
       <c r="H27" t="n">
-        <v>0.001109199</v>
+        <v>0.029744094590026</v>
       </c>
       <c r="I27" t="n">
         <v>-0.1523297439645124</v>
@@ -6187,7 +6187,7 @@
         <v>1.018325530689699</v>
       </c>
       <c r="C28" t="n">
-        <v>0.004073645633316419</v>
+        <v>0.00564497369026703</v>
       </c>
       <c r="D28" t="n">
         <v>-0.1522435997185894</v>
@@ -6202,7 +6202,7 @@
         <v>5.579</v>
       </c>
       <c r="H28" t="n">
-        <v>0.001115731</v>
+        <v>0.021438499750743</v>
       </c>
       <c r="I28" t="n">
         <v>-0.1522435997185894</v>
@@ -6221,7 +6221,7 @@
         <v>1.017669872079825</v>
       </c>
       <c r="C29" t="n">
-        <v>0.002761032464980853</v>
+        <v>0.003918433982497729</v>
       </c>
       <c r="D29" t="n">
         <v>-0.1516284990597248</v>
@@ -6236,7 +6236,7 @@
         <v>5.573</v>
       </c>
       <c r="H29" t="n">
-        <v>0.001114655</v>
+        <v>0.015267067986888</v>
       </c>
       <c r="I29" t="n">
         <v>-0.1516284990597248</v>
@@ -6255,7 +6255,7 @@
         <v>1.018213012197017</v>
       </c>
       <c r="C30" t="n">
-        <v>0.003163649795984415</v>
+        <v>0.004429348111081433</v>
       </c>
       <c r="D30" t="n">
         <v>-0.1523040484881624</v>
@@ -6270,7 +6270,7 @@
         <v>5.57</v>
       </c>
       <c r="H30" t="n">
-        <v>0.00111397</v>
+        <v>0.016995081270198</v>
       </c>
       <c r="I30" t="n">
         <v>-0.1523040484881624</v>
@@ -6289,7 +6289,7 @@
         <v>1.017740064549845</v>
       </c>
       <c r="C31" t="n">
-        <v>0.003090647901958218</v>
+        <v>0.004162510627696204</v>
       </c>
       <c r="D31" t="n">
         <v>-0.1517500518851931</v>
@@ -6304,7 +6304,7 @@
         <v>5.575</v>
       </c>
       <c r="H31" t="n">
-        <v>0.001115018</v>
+        <v>0.015314237193869</v>
       </c>
       <c r="I31" t="n">
         <v>-0.1517500518851931</v>
@@ -6323,7 +6323,7 @@
         <v>1.016881802964801</v>
       </c>
       <c r="C32" t="n">
-        <v>0.002517404189356286</v>
+        <v>0.003400473994618108</v>
       </c>
       <c r="D32" t="n">
         <v>-0.1894688903953767</v>
@@ -6338,7 +6338,7 @@
         <v>5.596</v>
       </c>
       <c r="H32" t="n">
-        <v>0.001119259</v>
+        <v>0.012629898170336</v>
       </c>
       <c r="I32" t="n">
         <v>-0.1894688903953767</v>
@@ -6357,7 +6357,7 @@
         <v>1.016443709258752</v>
       </c>
       <c r="C33" t="n">
-        <v>0.003505712878289714</v>
+        <v>0.004292355322701152</v>
       </c>
       <c r="D33" t="n">
         <v>-0.1893762681164637</v>
@@ -6372,7 +6372,7 @@
         <v>5.57</v>
       </c>
       <c r="H33" t="n">
-        <v>0.001113944</v>
+        <v>0.013617955788718</v>
       </c>
       <c r="I33" t="n">
         <v>-0.1893762681164637</v>
@@ -6391,7 +6391,7 @@
         <v>1.016767628922006</v>
       </c>
       <c r="C34" t="n">
-        <v>0.002421107806708582</v>
+        <v>0.003289246279646641</v>
       </c>
       <c r="D34" t="n">
         <v>-0.1899022828866734</v>
@@ -6406,7 +6406,7 @@
         <v>5.594</v>
       </c>
       <c r="H34" t="n">
-        <v>0.001118735</v>
+        <v>0.012300716631549</v>
       </c>
       <c r="I34" t="n">
         <v>-0.1899022828866734</v>
@@ -6425,7 +6425,7 @@
         <v>1.016683512507745</v>
       </c>
       <c r="C35" t="n">
-        <v>0.002710059438792958</v>
+        <v>0.003828105769477187</v>
       </c>
       <c r="D35" t="n">
         <v>-0.1897262701136946</v>
@@ -6440,7 +6440,7 @@
         <v>5.592</v>
       </c>
       <c r="H35" t="n">
-        <v>0.001118395</v>
+        <v>0.014912963650047</v>
       </c>
       <c r="I35" t="n">
         <v>-0.1897262701136946</v>
@@ -6459,7 +6459,7 @@
         <v>1.016992201397093</v>
       </c>
       <c r="C36" t="n">
-        <v>0.002476498359863639</v>
+        <v>0.00404754222426729</v>
       </c>
       <c r="D36" t="n">
         <v>-0.1897733691051613</v>
@@ -6474,7 +6474,7 @@
         <v>5.596</v>
       </c>
       <c r="H36" t="n">
-        <v>0.001119128</v>
+        <v>0.017651725874693</v>
       </c>
       <c r="I36" t="n">
         <v>-0.1897733691051613</v>
@@ -6493,7 +6493,7 @@
         <v>1.016985494451034</v>
       </c>
       <c r="C37" t="n">
-        <v>0.003333709501632135</v>
+        <v>0.005041366938133791</v>
       </c>
       <c r="D37" t="n">
         <v>-0.1899356200044511</v>
@@ -6508,7 +6508,7 @@
         <v>5.571</v>
       </c>
       <c r="H37" t="n">
-        <v>0.001114252</v>
+        <v>0.020746290517999</v>
       </c>
       <c r="I37" t="n">
         <v>-0.1899356200044511</v>
@@ -6527,7 +6527,7 @@
         <v>1.016476989247063</v>
       </c>
       <c r="C38" t="n">
-        <v>0.003069688421780098</v>
+        <v>0.004409176775394881</v>
       </c>
       <c r="D38" t="n">
         <v>-0.1898097927036959</v>
@@ -6542,7 +6542,7 @@
         <v>5.593</v>
       </c>
       <c r="H38" t="n">
-        <v>0.001118636</v>
+        <v>0.017451334974756</v>
       </c>
       <c r="I38" t="n">
         <v>-0.1898097927036959</v>
@@ -6561,7 +6561,7 @@
         <v>1.017032160321141</v>
       </c>
       <c r="C39" t="n">
-        <v>0.002690369349173385</v>
+        <v>0.003811395046518484</v>
       </c>
       <c r="D39" t="n">
         <v>-0.1900993259780035</v>
@@ -6576,7 +6576,7 @@
         <v>5.581</v>
       </c>
       <c r="H39" t="n">
-        <v>0.001116173</v>
+        <v>0.014856955800656</v>
       </c>
       <c r="I39" t="n">
         <v>-0.1900993259780035</v>
@@ -6595,7 +6595,7 @@
         <v>1.016991791201618</v>
       </c>
       <c r="C40" t="n">
-        <v>0.002358273030176507</v>
+        <v>0.003220610439917267</v>
       </c>
       <c r="D40" t="n">
         <v>-0.1901219848709348</v>
@@ -6610,7 +6610,7 @@
         <v>5.59</v>
       </c>
       <c r="H40" t="n">
-        <v>0.00111793</v>
+        <v>0.012107814239987</v>
       </c>
       <c r="I40" t="n">
         <v>-0.1901219848709348</v>
@@ -6629,7 +6629,7 @@
         <v>1.01677167320184</v>
       </c>
       <c r="C41" t="n">
-        <v>0.002103378256928673</v>
+        <v>0.002403736411786261</v>
       </c>
       <c r="D41" t="n">
         <v>-0.189423168809548</v>
@@ -6644,7 +6644,7 @@
         <v>5.586</v>
       </c>
       <c r="H41" t="n">
-        <v>0.00111722</v>
+        <v>0.006489042918398</v>
       </c>
       <c r="I41" t="n">
         <v>-0.189423168809548</v>
@@ -6663,7 +6663,7 @@
         <v>1.015287530429565</v>
       </c>
       <c r="C42" t="n">
-        <v>0.002275882137218842</v>
+        <v>0.003111998737711569</v>
       </c>
       <c r="D42" t="n">
         <v>-0.2371998859887468</v>
@@ -6678,7 +6678,7 @@
         <v>11.28</v>
       </c>
       <c r="H42" t="n">
-        <v>0.002256042</v>
+        <v>0.023688687446238</v>
       </c>
       <c r="I42" t="n">
         <v>-0.2371998859887468</v>
@@ -6697,7 +6697,7 @@
         <v>1.015507185881661</v>
       </c>
       <c r="C43" t="n">
-        <v>0.00203233755083447</v>
+        <v>0.002949415411475437</v>
       </c>
       <c r="D43" t="n">
         <v>-0.2374395802762082</v>
@@ -6712,7 +6712,7 @@
         <v>11.272</v>
       </c>
       <c r="H43" t="n">
-        <v>0.002254355</v>
+        <v>0.023832187938277</v>
       </c>
       <c r="I43" t="n">
         <v>-0.2374395802762082</v>
@@ -6731,7 +6731,7 @@
         <v>1.015401747564822</v>
       </c>
       <c r="C44" t="n">
-        <v>0.002180257135799891</v>
+        <v>0.003249768325906804</v>
       </c>
       <c r="D44" t="n">
         <v>-0.2372800976627194</v>
@@ -6746,7 +6746,7 @@
         <v>11.273</v>
       </c>
       <c r="H44" t="n">
-        <v>0.002254673</v>
+        <v>0.026849234947934</v>
       </c>
       <c r="I44" t="n">
         <v>-0.2372800976627194</v>
@@ -6765,7 +6765,7 @@
         <v>1.0155538649882</v>
       </c>
       <c r="C45" t="n">
-        <v>0.002383383929122085</v>
+        <v>0.003369572833881639</v>
       </c>
       <c r="D45" t="n">
         <v>-0.2377231390478642</v>
@@ -6780,7 +6780,7 @@
         <v>11.272</v>
       </c>
       <c r="H45" t="n">
-        <v>0.002254388</v>
+        <v>0.026533641107474</v>
       </c>
       <c r="I45" t="n">
         <v>-0.2377231390478642</v>
@@ -6799,7 +6799,7 @@
         <v>1.015218699552001</v>
       </c>
       <c r="C46" t="n">
-        <v>0.002065698100613004</v>
+        <v>0.002623207997502186</v>
       </c>
       <c r="D46" t="n">
         <v>-0.2366795655649319</v>
@@ -6814,7 +6814,7 @@
         <v>11.265</v>
       </c>
       <c r="H46" t="n">
-        <v>0.00225301</v>
+        <v>0.018081378963867</v>
       </c>
       <c r="I46" t="n">
         <v>-0.2366795655649319</v>
@@ -6833,7 +6833,7 @@
         <v>1.015376833937671</v>
       </c>
       <c r="C47" t="n">
-        <v>0.001798534864085495</v>
+        <v>0.002485810462870884</v>
       </c>
       <c r="D47" t="n">
         <v>-0.2374148109787018</v>
@@ -6848,7 +6848,7 @@
         <v>11.282</v>
       </c>
       <c r="H47" t="n">
-        <v>0.002256496</v>
+        <v>0.019199368989646</v>
       </c>
       <c r="I47" t="n">
         <v>-0.2374148109787018</v>
@@ -6867,7 +6867,7 @@
         <v>1.015282931577932</v>
       </c>
       <c r="C48" t="n">
-        <v>0.001857528762469348</v>
+        <v>0.002423027891007316</v>
       </c>
       <c r="D48" t="n">
         <v>-0.237054109419446</v>
@@ -6882,7 +6882,7 @@
         <v>11.282</v>
       </c>
       <c r="H48" t="n">
-        <v>0.002256465</v>
+        <v>0.017435440637342</v>
       </c>
       <c r="I48" t="n">
         <v>-0.237054109419446</v>
@@ -6901,7 +6901,7 @@
         <v>1.015083331313351</v>
       </c>
       <c r="C49" t="n">
-        <v>0.001776884298835166</v>
+        <v>0.002527783011691038</v>
       </c>
       <c r="D49" t="n">
         <v>-0.2366787429961543</v>
@@ -6916,7 +6916,7 @@
         <v>11.264</v>
       </c>
       <c r="H49" t="n">
-        <v>0.00225281</v>
+        <v>0.020077182874202</v>
       </c>
       <c r="I49" t="n">
         <v>-0.2366787429961543</v>
@@ -6935,7 +6935,7 @@
         <v>1.014817390689611</v>
       </c>
       <c r="C50" t="n">
-        <v>0.003028690216879394</v>
+        <v>0.003686403387753666</v>
       </c>
       <c r="D50" t="n">
         <v>-0.2365628466730563</v>
@@ -6950,7 +6950,7 @@
         <v>11.284</v>
       </c>
       <c r="H50" t="n">
-        <v>0.002256829</v>
+        <v>0.023476616326684</v>
       </c>
       <c r="I50" t="n">
         <v>-0.2365628466730563</v>
@@ -6969,7 +6969,7 @@
         <v>1.015285154307868</v>
       </c>
       <c r="C51" t="n">
-        <v>0.002646685685617881</v>
+        <v>0.003831003073481512</v>
       </c>
       <c r="D51" t="n">
         <v>-0.2373388303386905</v>
@@ -6984,7 +6984,7 @@
         <v>11.281</v>
       </c>
       <c r="H51" t="n">
-        <v>0.002256244</v>
+        <v>0.0308579917812</v>
       </c>
       <c r="I51" t="n">
         <v>-0.2373388303386905</v>
@@ -7003,7 +7003,7 @@
         <v>1.012798570405463</v>
       </c>
       <c r="C52" t="n">
-        <v>0.001317846985944281</v>
+        <v>0.001775381686142341</v>
       </c>
       <c r="D52" t="n">
         <v>-0.2987690391140281</v>
@@ -7018,7 +7018,7 @@
         <v>11.425</v>
       </c>
       <c r="H52" t="n">
-        <v>0.002285012</v>
+        <v>0.013613102380448</v>
       </c>
       <c r="I52" t="n">
         <v>-0.2987690391140281</v>
@@ -7037,7 +7037,7 @@
         <v>1.012732527434692</v>
       </c>
       <c r="C53" t="n">
-        <v>0.001579439874526018</v>
+        <v>0.002264132091516062</v>
       </c>
       <c r="D53" t="n">
         <v>-0.2986780078685594</v>
@@ -7052,7 +7052,7 @@
         <v>11.436</v>
       </c>
       <c r="H53" t="n">
-        <v>0.002287214</v>
+        <v>0.018460932450378</v>
       </c>
       <c r="I53" t="n">
         <v>-0.2986780078685594</v>
@@ -7071,7 +7071,7 @@
         <v>1.012643600138697</v>
       </c>
       <c r="C54" t="n">
-        <v>0.001390569541604939</v>
+        <v>0.00153937729937816</v>
       </c>
       <c r="D54" t="n">
         <v>-0.2985702850478891</v>
@@ -7086,7 +7086,7 @@
         <v>11.437</v>
       </c>
       <c r="H54" t="n">
-        <v>0.00228731</v>
+        <v>0.007800470922491</v>
       </c>
       <c r="I54" t="n">
         <v>-0.2985702850478891</v>
@@ -7105,7 +7105,7 @@
         <v>1.012746610054463</v>
       </c>
       <c r="C55" t="n">
-        <v>0.001471493274832445</v>
+        <v>0.001861551487294796</v>
       </c>
       <c r="D55" t="n">
         <v>-0.298823225309897</v>
@@ -7120,7 +7120,7 @@
         <v>11.427</v>
       </c>
       <c r="H55" t="n">
-        <v>0.00228542</v>
+        <v>0.013066623425462</v>
       </c>
       <c r="I55" t="n">
         <v>-0.298823225309897</v>
@@ -7139,7 +7139,7 @@
         <v>1.012805725212618</v>
       </c>
       <c r="C56" t="n">
-        <v>0.001287487584829475</v>
+        <v>0.001725431370878325</v>
       </c>
       <c r="D56" t="n">
         <v>-0.2989192184229506</v>
@@ -7154,7 +7154,7 @@
         <v>11.428</v>
       </c>
       <c r="H56" t="n">
-        <v>0.002285675</v>
+        <v>0.01316124589677</v>
       </c>
       <c r="I56" t="n">
         <v>-0.2989192184229506</v>
@@ -7173,7 +7173,7 @@
         <v>1.013319075603283</v>
       </c>
       <c r="C57" t="n">
-        <v>0.001935391162793501</v>
+        <v>0.002671146419412408</v>
       </c>
       <c r="D57" t="n">
         <v>-0.2995803928810874</v>
@@ -7188,7 +7188,7 @@
         <v>11.408</v>
       </c>
       <c r="H57" t="n">
-        <v>0.002281506</v>
+        <v>0.020851280528231</v>
       </c>
       <c r="I57" t="n">
         <v>-0.2995803928810874</v>
@@ -7207,7 +7207,7 @@
         <v>1.013309994471796</v>
       </c>
       <c r="C58" t="n">
-        <v>0.002775611203701994</v>
+        <v>0.003631402059539958</v>
       </c>
       <c r="D58" t="n">
         <v>-0.3003890740551816</v>
@@ -7222,7 +7222,7 @@
         <v>11.428</v>
       </c>
       <c r="H58" t="n">
-        <v>0.002285501</v>
+        <v>0.026506959661577</v>
       </c>
       <c r="I58" t="n">
         <v>-0.3003890740551816</v>
@@ -7241,7 +7241,7 @@
         <v>1.013213696022409</v>
       </c>
       <c r="C59" t="n">
-        <v>0.00134686692720598</v>
+        <v>0.001579936413638478</v>
       </c>
       <c r="D59" t="n">
         <v>-0.2996998233577313</v>
@@ -7256,7 +7256,7 @@
         <v>11.421</v>
       </c>
       <c r="H59" t="n">
-        <v>0.002284136</v>
+        <v>0.009585955096397</v>
       </c>
       <c r="I59" t="n">
         <v>-0.2996998233577313</v>
@@ -7275,7 +7275,7 @@
         <v>1.012786753961046</v>
       </c>
       <c r="C60" t="n">
-        <v>0.001394466215983616</v>
+        <v>0.001909446613721145</v>
       </c>
       <c r="D60" t="n">
         <v>-0.2989371966815226</v>
@@ -7290,7 +7290,7 @@
         <v>11.432</v>
       </c>
       <c r="H60" t="n">
-        <v>0.002286365</v>
+        <v>0.014900056855581</v>
       </c>
       <c r="I60" t="n">
         <v>-0.2989371966815226</v>
@@ -7309,7 +7309,7 @@
         <v>1.012777492710821</v>
       </c>
       <c r="C61" t="n">
-        <v>0.001235051607266392</v>
+        <v>0.001511854389866237</v>
       </c>
       <c r="D61" t="n">
         <v>-0.2986611663022831</v>
@@ -7324,7 +7324,7 @@
         <v>11.441</v>
       </c>
       <c r="H61" t="n">
-        <v>0.002288201</v>
+        <v>0.010112748140394</v>
       </c>
       <c r="I61" t="n">
         <v>-0.2986611663022831</v>
@@ -7343,7 +7343,7 @@
         <v>1.008743004541071</v>
       </c>
       <c r="C62" t="n">
-        <v>0.000618909021383461</v>
+        <v>0.0007494624379731547</v>
       </c>
       <c r="D62" t="n">
         <v>-0.3793909902467334</v>
@@ -7358,7 +7358,7 @@
         <v>23.243</v>
       </c>
       <c r="H62" t="n">
-        <v>0.00464855</v>
+        <v>0.01079139738391</v>
       </c>
       <c r="I62" t="n">
         <v>-0.3793909902467334</v>
@@ -7377,7 +7377,7 @@
         <v>1.0087959486256</v>
       </c>
       <c r="C63" t="n">
-        <v>0.0005130120482461199</v>
+        <v>0.000631847309226144</v>
       </c>
       <c r="D63" t="n">
         <v>-0.3796630766128217</v>
@@ -7392,7 +7392,7 @@
         <v>23.252</v>
       </c>
       <c r="H63" t="n">
-        <v>0.004650455</v>
+        <v>0.009690490941299</v>
       </c>
       <c r="I63" t="n">
         <v>-0.3796630766128217</v>
@@ -7411,7 +7411,7 @@
         <v>1.008848307172733</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0004799887246263073</v>
+        <v>0.0004946007550755803</v>
       </c>
       <c r="D64" t="n">
         <v>-0.38014006893932</v>
@@ -7426,7 +7426,7 @@
         <v>23.245</v>
       </c>
       <c r="H64" t="n">
-        <v>0.004649079</v>
+        <v>0.005401318945188</v>
       </c>
       <c r="I64" t="n">
         <v>-0.38014006893932</v>
@@ -7445,7 +7445,7 @@
         <v>1.008880806262734</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0007152510191612711</v>
+        <v>0.0008250297171524787</v>
       </c>
       <c r="D65" t="n">
         <v>-0.3806289309495394</v>
@@ -7460,7 +7460,7 @@
         <v>23.237</v>
       </c>
       <c r="H65" t="n">
-        <v>0.004647441</v>
+        <v>0.010549878156922</v>
       </c>
       <c r="I65" t="n">
         <v>-0.3806289309495394</v>
@@ -7479,7 +7479,7 @@
         <v>1.008767253431289</v>
       </c>
       <c r="C66" t="n">
-        <v>0.0004589046753223188</v>
+        <v>0.0004492126807884262</v>
       </c>
       <c r="D66" t="n">
         <v>-0.3796467833670958</v>
@@ -7494,7 +7494,7 @@
         <v>23.24</v>
       </c>
       <c r="H66" t="n">
-        <v>0.00464804</v>
+        <v>0.00411495969702</v>
       </c>
       <c r="I66" t="n">
         <v>-0.3796467833670958</v>
@@ -7513,7 +7513,7 @@
         <v>1.008800123212527</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0006043842282571993</v>
+        <v>0.0007897458160709573</v>
       </c>
       <c r="D67" t="n">
         <v>-0.3798326866942965</v>
@@ -7528,7 +7528,7 @@
         <v>23.242</v>
       </c>
       <c r="H67" t="n">
-        <v>0.004648389</v>
+        <v>0.012600703119181</v>
       </c>
       <c r="I67" t="n">
         <v>-0.3798326866942965</v>
@@ -7547,7 +7547,7 @@
         <v>1.008819087953056</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0004953411539011634</v>
+        <v>0.0005394320628079545</v>
       </c>
       <c r="D68" t="n">
         <v>-0.3796860475339305</v>
@@ -7562,7 +7562,7 @@
         <v>23.251</v>
       </c>
       <c r="H68" t="n">
-        <v>0.0046502</v>
+        <v>0.006771986468694</v>
       </c>
       <c r="I68" t="n">
         <v>-0.3796860475339305</v>
@@ -7581,7 +7581,7 @@
         <v>1.008947717669804</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0007834326876717969</v>
+        <v>0.001020735413561813</v>
       </c>
       <c r="D69" t="n">
         <v>-0.379098896239479</v>
@@ -7596,7 +7596,7 @@
         <v>23.261</v>
       </c>
       <c r="H69" t="n">
-        <v>0.004652268</v>
+        <v>0.015786237524833</v>
       </c>
       <c r="I69" t="n">
         <v>-0.379098896239479</v>
@@ -7615,7 +7615,7 @@
         <v>1.008915434191853</v>
       </c>
       <c r="C70" t="n">
-        <v>0.000732735977403343</v>
+        <v>0.0008967195452835347</v>
       </c>
       <c r="D70" t="n">
         <v>-0.3802869488155958</v>
@@ -7630,7 +7630,7 @@
         <v>23.248</v>
       </c>
       <c r="H70" t="n">
-        <v>0.004649516</v>
+        <v>0.0127864205841</v>
       </c>
       <c r="I70" t="n">
         <v>-0.3802869488155958</v>
@@ -7649,7 +7649,7 @@
         <v>1.008898780563483</v>
       </c>
       <c r="C71" t="n">
-        <v>0.0006247134220685095</v>
+        <v>0.0007761383951578342</v>
       </c>
       <c r="D71" t="n">
         <v>-0.3798335801087296</v>
@@ -7664,7 +7664,7 @@
         <v>23.245</v>
       </c>
       <c r="H71" t="n">
-        <v>0.004648937</v>
+        <v>0.01158518714659</v>
       </c>
       <c r="I71" t="n">
         <v>-0.3798335801087296</v>
@@ -7683,7 +7683,7 @@
         <v>1.005107399069952</v>
       </c>
       <c r="C72" t="n">
-        <v>0.0006938924553663514</v>
+        <v>0.0009634622934971437</v>
       </c>
       <c r="D72" t="n">
         <v>-0.4432829053829517</v>
@@ -7698,7 +7698,7 @@
         <v>58.508</v>
       </c>
       <c r="H72" t="n">
-        <v>0.011701683</v>
+        <v>0.040630191766092</v>
       </c>
       <c r="I72" t="n">
         <v>-0.4432829053829517</v>
@@ -7717,7 +7717,7 @@
         <v>1.005098519074723</v>
       </c>
       <c r="C73" t="n">
-        <v>0.0007449078710313631</v>
+        <v>0.0009388164204812917</v>
       </c>
       <c r="D73" t="n">
         <v>-0.4431887334387503</v>
@@ -7732,7 +7732,7 @@
         <v>58.504</v>
       </c>
       <c r="H73" t="n">
-        <v>0.01170086</v>
+        <v>0.03525733832011</v>
       </c>
       <c r="I73" t="n">
         <v>-0.4431887334387503</v>
@@ -7751,7 +7751,7 @@
         <v>1.00503804030251</v>
       </c>
       <c r="C74" t="n">
-        <v>0.0005730189609135099</v>
+        <v>0.0007420718290303581</v>
       </c>
       <c r="D74" t="n">
         <v>-0.4436922790960365</v>
@@ -7766,7 +7766,7 @@
         <v>58.523</v>
       </c>
       <c r="H74" t="n">
-        <v>0.011704522</v>
+        <v>0.029846502762783</v>
       </c>
       <c r="I74" t="n">
         <v>-0.4436922790960365</v>
@@ -7785,7 +7785,7 @@
         <v>1.004971440676563</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0009110726529398588</v>
+        <v>0.001292484342835764</v>
       </c>
       <c r="D75" t="n">
         <v>-0.4440611706876556</v>
@@ -7800,7 +7800,7 @@
         <v>58.496</v>
       </c>
       <c r="H75" t="n">
-        <v>0.011699189</v>
+        <v>0.054629364308104</v>
       </c>
       <c r="I75" t="n">
         <v>-0.4440611706876556</v>
@@ -7819,7 +7819,7 @@
         <v>1.004886720036684</v>
       </c>
       <c r="C76" t="n">
-        <v>0.0008939251019939975</v>
+        <v>0.001134455368611055</v>
       </c>
       <c r="D76" t="n">
         <v>-0.4448773254100908</v>
@@ -7834,7 +7834,7 @@
         <v>58.55</v>
       </c>
       <c r="H76" t="n">
-        <v>0.011709924</v>
+        <v>0.04234880534878</v>
       </c>
       <c r="I76" t="n">
         <v>-0.4448773254100908</v>
@@ -7853,7 +7853,7 @@
         <v>1.005158721225767</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0008666352545804811</v>
+        <v>0.00107331028249475</v>
       </c>
       <c r="D77" t="n">
         <v>-0.4428157179747494</v>
@@ -7868,7 +7868,7 @@
         <v>58.496</v>
       </c>
       <c r="H77" t="n">
-        <v>0.011699266</v>
+        <v>0.038662001025846</v>
       </c>
       <c r="I77" t="n">
         <v>-0.4428157179747494</v>
@@ -7887,7 +7887,7 @@
         <v>1.00504248163198</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0005811448184493322</v>
+        <v>0.0007384507995522497</v>
       </c>
       <c r="D78" t="n">
         <v>-0.4435049172289358</v>
@@ -7902,7 +7902,7 @@
         <v>58.499</v>
       </c>
       <c r="H78" t="n">
-        <v>0.011699812</v>
+        <v>0.028985215800893</v>
       </c>
       <c r="I78" t="n">
         <v>-0.4435049172289358</v>
@@ -7921,7 +7921,7 @@
         <v>1.005142061184867</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0005693971787223368</v>
+        <v>0.0008074708578920156</v>
       </c>
       <c r="D79" t="n">
         <v>-0.4441734776141759</v>
@@ -7936,7 +7936,7 @@
         <v>58.641</v>
       </c>
       <c r="H79" t="n">
-        <v>0.011728122</v>
+        <v>0.035401403994845</v>
       </c>
       <c r="I79" t="n">
         <v>-0.4441734776141759</v>
@@ -7955,7 +7955,7 @@
         <v>1.005186741502615</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0005454115884150253</v>
+        <v>0.0007263126191858004</v>
       </c>
       <c r="D80" t="n">
         <v>-0.4433168180520348</v>
@@ -7970,7 +7970,7 @@
         <v>58.593</v>
       </c>
       <c r="H80" t="n">
-        <v>0.011718531</v>
+        <v>0.030315165691413</v>
       </c>
       <c r="I80" t="n">
         <v>-0.4433168180520348</v>
@@ -7989,7 +7989,7 @@
         <v>1.005031494570573</v>
       </c>
       <c r="C81" t="n">
-        <v>0.0007623566128473175</v>
+        <v>0.00112939510806512</v>
       </c>
       <c r="D81" t="n">
         <v>-0.4441091353740227</v>
@@ -8004,7 +8004,7 @@
         <v>58.579</v>
       </c>
       <c r="H81" t="n">
-        <v>0.011715724</v>
+        <v>0.049961066345617</v>
       </c>
       <c r="I81" t="n">
         <v>-0.4441091353740227</v>
@@ -8023,7 +8023,7 @@
         <v>1.003008962794092</v>
       </c>
       <c r="C82" t="n">
-        <v>0.001195208795783718</v>
+        <v>0.001609392068872857</v>
       </c>
       <c r="D82" t="n">
         <v>-0.4737995664330619</v>
@@ -8038,7 +8038,7 @@
         <v>58.703</v>
       </c>
       <c r="H82" t="n">
-        <v>0.011740505</v>
+        <v>0.064162647768314</v>
       </c>
       <c r="I82" t="n">
         <v>-0.4737995664330619</v>
@@ -8057,7 +8057,7 @@
         <v>1.002856263815213</v>
       </c>
       <c r="C83" t="n">
-        <v>0.0006628116990986085</v>
+        <v>0.0008667336583044521</v>
       </c>
       <c r="D83" t="n">
         <v>-0.4749359970228033</v>
@@ -8072,7 +8072,7 @@
         <v>58.766</v>
       </c>
       <c r="H83" t="n">
-        <v>0.01175327</v>
+        <v>0.034773098287822</v>
       </c>
       <c r="I83" t="n">
         <v>-0.4749359970228033</v>
@@ -8091,7 +8091,7 @@
         <v>1.002948091020979</v>
       </c>
       <c r="C84" t="n">
-        <v>0.0008132357011881613</v>
+        <v>0.001052185731552099</v>
       </c>
       <c r="D84" t="n">
         <v>-0.4741788883501683</v>
@@ -8106,7 +8106,7 @@
         <v>58.718</v>
       </c>
       <c r="H84" t="n">
-        <v>0.011743551</v>
+        <v>0.040813258253252</v>
       </c>
       <c r="I84" t="n">
         <v>-0.4741788883501683</v>
@@ -8125,7 +8125,7 @@
         <v>1.003101970502895</v>
       </c>
       <c r="C85" t="n">
-        <v>0.001447757567339947</v>
+        <v>0.001962139329765276</v>
       </c>
       <c r="D85" t="n">
         <v>-0.4734197171541923</v>
@@ -8140,7 +8140,7 @@
         <v>58.717</v>
       </c>
       <c r="H85" t="n">
-        <v>0.011743445</v>
+        <v>0.07840770725506201</v>
       </c>
       <c r="I85" t="n">
         <v>-0.4734197171541923</v>
@@ -8159,7 +8159,7 @@
         <v>1.002843934701599</v>
       </c>
       <c r="C86" t="n">
-        <v>0.0006089208175329934</v>
+        <v>0.0008934795939425894</v>
       </c>
       <c r="D86" t="n">
         <v>-0.4747106782280412</v>
@@ -8174,7 +8174,7 @@
         <v>58.763</v>
       </c>
       <c r="H86" t="n">
-        <v>0.011752671</v>
+        <v>0.040075347341541</v>
       </c>
       <c r="I86" t="n">
         <v>-0.4747106782280412</v>
@@ -8193,7 +8193,7 @@
         <v>1.002991023267885</v>
       </c>
       <c r="C87" t="n">
-        <v>0.0008015285676968817</v>
+        <v>0.0008750309577018272</v>
       </c>
       <c r="D87" t="n">
         <v>-0.4740426902533468</v>
@@ -8208,7 +8208,7 @@
         <v>58.731</v>
       </c>
       <c r="H87" t="n">
-        <v>0.011746171</v>
+        <v>0.023675008415263</v>
       </c>
       <c r="I87" t="n">
         <v>-0.4740426902533468</v>
@@ -8227,7 +8227,7 @@
         <v>1.002820704358146</v>
       </c>
       <c r="C88" t="n">
-        <v>0.0008044732315429368</v>
+        <v>0.001174555667443932</v>
       </c>
       <c r="D88" t="n">
         <v>-0.4747647576397078</v>
@@ -8242,7 +8242,7 @@
         <v>58.737</v>
       </c>
       <c r="H88" t="n">
-        <v>0.011747443</v>
+        <v>0.051484237162339</v>
       </c>
       <c r="I88" t="n">
         <v>-0.4747647576397078</v>
@@ -8261,7 +8261,7 @@
         <v>1.002944764019071</v>
       </c>
       <c r="C89" t="n">
-        <v>0.0009772441830977262</v>
+        <v>0.001432590956392371</v>
       </c>
       <c r="D89" t="n">
         <v>-0.4749757376033585</v>
@@ -8276,7 +8276,7 @@
         <v>58.916</v>
       </c>
       <c r="H89" t="n">
-        <v>0.011783128</v>
+        <v>0.062652836729364</v>
       </c>
       <c r="I89" t="n">
         <v>-0.4749757376033585</v>
@@ -8295,7 +8295,7 @@
         <v>1.002898128664435</v>
       </c>
       <c r="C90" t="n">
-        <v>0.0008015352464668286</v>
+        <v>0.001076815579841178</v>
       </c>
       <c r="D90" t="n">
         <v>-0.4748442727500737</v>
@@ -8310,7 +8310,7 @@
         <v>58.822</v>
       </c>
       <c r="H90" t="n">
-        <v>0.011764438</v>
+        <v>0.043785430661915</v>
       </c>
       <c r="I90" t="n">
         <v>-0.4748442727500737</v>
@@ -8329,7 +8329,7 @@
         <v>1.002977583220767</v>
       </c>
       <c r="C91" t="n">
-        <v>0.0006075181167209473</v>
+        <v>0.0007110946044478605</v>
       </c>
       <c r="D91" t="n">
         <v>-0.4741270289349737</v>
@@ -8344,7 +8344,7 @@
         <v>58.708</v>
       </c>
       <c r="H91" t="n">
-        <v>0.011741662</v>
+        <v>0.02461314781147</v>
       </c>
       <c r="I91" t="n">
         <v>-0.4741270289349737</v>
@@ -8363,7 +8363,7 @@
         <v>1.00030247871122</v>
       </c>
       <c r="C92" t="n">
-        <v>0.001016751950319031</v>
+        <v>0.001296822644691311</v>
       </c>
       <c r="D92" t="n">
         <v>-0.5071334051566674</v>
@@ -8378,7 +8378,7 @@
         <v>59.176</v>
       </c>
       <c r="H92" t="n">
-        <v>0.011835273</v>
+        <v>0.049068756457295</v>
       </c>
       <c r="I92" t="n">
         <v>-0.5071334051566674</v>
@@ -8397,7 +8397,7 @@
         <v>1.000601742357886</v>
       </c>
       <c r="C93" t="n">
-        <v>0.000705473856335205</v>
+        <v>0.0009639183623541758</v>
       </c>
       <c r="D93" t="n">
         <v>-0.5062970902106931</v>
@@ -8412,7 +8412,7 @@
         <v>59.13</v>
       </c>
       <c r="H93" t="n">
-        <v>0.011826076</v>
+        <v>0.040577442474431</v>
       </c>
       <c r="I93" t="n">
         <v>-0.5062970902106931</v>
@@ -8431,7 +8431,7 @@
         <v>1.000416723284994</v>
       </c>
       <c r="C94" t="n">
-        <v>0.001102022451582698</v>
+        <v>0.001512740351254498</v>
       </c>
       <c r="D94" t="n">
         <v>-0.5065916404885544</v>
@@ -8446,7 +8446,7 @@
         <v>59.085</v>
       </c>
       <c r="H94" t="n">
-        <v>0.011817012</v>
+        <v>0.062334968009377</v>
       </c>
       <c r="I94" t="n">
         <v>-0.5065916404885544</v>
@@ -8465,7 +8465,7 @@
         <v>1.000442435622856</v>
       </c>
       <c r="C95" t="n">
-        <v>0.00127885797659287</v>
+        <v>0.001952303975614754</v>
       </c>
       <c r="D95" t="n">
         <v>-0.5063865216671704</v>
@@ -8480,7 +8480,7 @@
         <v>59.046</v>
       </c>
       <c r="H95" t="n">
-        <v>0.011809138</v>
+        <v>0.087859345931808</v>
       </c>
       <c r="I95" t="n">
         <v>-0.5063865216671704</v>
@@ -8499,7 +8499,7 @@
         <v>1.000713208568959</v>
       </c>
       <c r="C96" t="n">
-        <v>0.001295209350263033</v>
+        <v>0.001623120730379246</v>
       </c>
       <c r="D96" t="n">
         <v>-0.5054276178447537</v>
@@ -8514,7 +8514,7 @@
         <v>58.992</v>
       </c>
       <c r="H96" t="n">
-        <v>0.011798353</v>
+        <v>0.058861772099815</v>
       </c>
       <c r="I96" t="n">
         <v>-0.5054276178447537</v>
@@ -8533,7 +8533,7 @@
         <v>1.000740015621597</v>
       </c>
       <c r="C97" t="n">
-        <v>0.00181348687971633</v>
+        <v>0.002773089668477631</v>
       </c>
       <c r="D97" t="n">
         <v>-0.505865278335131</v>
@@ -8548,7 +8548,7 @@
         <v>59.286</v>
       </c>
       <c r="H97" t="n">
-        <v>0.011857186</v>
+        <v>0.124849963939319</v>
       </c>
       <c r="I97" t="n">
         <v>-0.505865278335131</v>
@@ -8567,7 +8567,7 @@
         <v>1.000677724758322</v>
       </c>
       <c r="C98" t="n">
-        <v>0.0007664184776829521</v>
+        <v>0.0009889300934574155</v>
       </c>
       <c r="D98" t="n">
         <v>-0.5056590382522268</v>
@@ -8582,7 +8582,7 @@
         <v>59.085</v>
       </c>
       <c r="H98" t="n">
-        <v>0.011817045</v>
+        <v>0.038747187551433</v>
       </c>
       <c r="I98" t="n">
         <v>-0.5056590382522268</v>
@@ -8601,7 +8601,7 @@
         <v>1.000507128380559</v>
       </c>
       <c r="C99" t="n">
-        <v>0.0008917972066861384</v>
+        <v>0.001223551171140559</v>
       </c>
       <c r="D99" t="n">
         <v>-0.5061927284693635</v>
@@ -8616,7 +8616,7 @@
         <v>59.062</v>
       </c>
       <c r="H99" t="n">
-        <v>0.011812307</v>
+        <v>0.050843543935493</v>
       </c>
       <c r="I99" t="n">
         <v>-0.5061927284693635</v>
@@ -8635,7 +8635,7 @@
         <v>1.000608541474318</v>
       </c>
       <c r="C100" t="n">
-        <v>0.001154449425608166</v>
+        <v>0.00174879773373412</v>
       </c>
       <c r="D100" t="n">
         <v>-0.5056735641900763</v>
@@ -8650,7 +8650,7 @@
         <v>59.024</v>
       </c>
       <c r="H100" t="n">
-        <v>0.011804889</v>
+        <v>0.078380725852827</v>
       </c>
       <c r="I100" t="n">
         <v>-0.5056735641900763</v>
@@ -8669,7 +8669,7 @@
         <v>1.000435579192966</v>
       </c>
       <c r="C101" t="n">
-        <v>0.000802603733420683</v>
+        <v>0.00113612862004408</v>
       </c>
       <c r="D101" t="n">
         <v>-0.5064506136142399</v>
@@ -8684,7 +8684,7 @@
         <v>59.037</v>
       </c>
       <c r="H101" t="n">
-        <v>0.011807354</v>
+        <v>0.048899326077849</v>
       </c>
       <c r="I101" t="n">
         <v>-0.5064506136142399</v>
@@ -8703,7 +8703,7 @@
         <v>0.9939434667755147</v>
       </c>
       <c r="C102" t="n">
-        <v>0.003653134965881874</v>
+        <v>0.005059305015985864</v>
       </c>
       <c r="D102" t="n">
         <v>-0.5976971218334075</v>
@@ -8718,7 +8718,7 @@
         <v>115.251</v>
       </c>
       <c r="H102" t="n">
-        <v>0.02305018</v>
+        <v>0.406509907208978</v>
       </c>
       <c r="I102" t="n">
         <v>-0.5976971218334075</v>
@@ -8737,7 +8737,7 @@
         <v>0.9935461577843577</v>
       </c>
       <c r="C103" t="n">
-        <v>0.001831817407153226</v>
+        <v>0.00263927973036725</v>
       </c>
       <c r="D103" t="n">
         <v>-0.598307882922839</v>
@@ -8752,7 +8752,7 @@
         <v>115.436</v>
       </c>
       <c r="H103" t="n">
-        <v>0.023087275</v>
+        <v>0.221964477449765</v>
       </c>
       <c r="I103" t="n">
         <v>-0.598307882922839</v>
@@ -8771,7 +8771,7 @@
         <v>0.993996073970748</v>
       </c>
       <c r="C104" t="n">
-        <v>0.00311724582444718</v>
+        <v>0.00409838491489138</v>
       </c>
       <c r="D104" t="n">
         <v>-0.5976911990363138</v>
@@ -8786,7 +8786,7 @@
         <v>115.693</v>
       </c>
       <c r="H104" t="n">
-        <v>0.023138529</v>
+        <v>0.310551540160933</v>
       </c>
       <c r="I104" t="n">
         <v>-0.5976911990363138</v>
@@ -8805,7 +8805,7 @@
         <v>0.9938830985744908</v>
       </c>
       <c r="C105" t="n">
-        <v>0.002926454872046902</v>
+        <v>0.003618202344607706</v>
       </c>
       <c r="D105" t="n">
         <v>-0.5977550400612124</v>
@@ -8820,7 +8820,7 @@
         <v>115.323</v>
       </c>
       <c r="H105" t="n">
-        <v>0.023064556</v>
+        <v>0.247961822365139</v>
       </c>
       <c r="I105" t="n">
         <v>-0.5977550400612124</v>
@@ -8839,7 +8839,7 @@
         <v>0.9944590423837842</v>
       </c>
       <c r="C106" t="n">
-        <v>0.005157415741780886</v>
+        <v>0.006655130665980841</v>
       </c>
       <c r="D106" t="n">
         <v>-0.597071998626868</v>
@@ -8854,7 +8854,7 @@
         <v>115.886</v>
       </c>
       <c r="H106" t="n">
-        <v>0.023177237</v>
+        <v>0.490699260015589</v>
       </c>
       <c r="I106" t="n">
         <v>-0.597071998626868</v>
@@ -8873,7 +8873,7 @@
         <v>0.9942926483548257</v>
       </c>
       <c r="C107" t="n">
-        <v>0.004453306542905417</v>
+        <v>0.005586832062975373</v>
       </c>
       <c r="D107" t="n">
         <v>-0.597142226360595</v>
@@ -8888,7 +8888,7 @@
         <v>115.264</v>
       </c>
       <c r="H107" t="n">
-        <v>0.023052821</v>
+        <v>0.391758275291741</v>
       </c>
       <c r="I107" t="n">
         <v>-0.597142226360595</v>
@@ -8907,7 +8907,7 @@
         <v>0.9937210820841557</v>
       </c>
       <c r="C108" t="n">
-        <v>0.002899864988146195</v>
+        <v>0.003686825695156925</v>
       </c>
       <c r="D108" t="n">
         <v>-0.5979441024274195</v>
@@ -8922,7 +8922,7 @@
         <v>115.091</v>
       </c>
       <c r="H108" t="n">
-        <v>0.023018107</v>
+        <v>0.264688728012457</v>
       </c>
       <c r="I108" t="n">
         <v>-0.5979441024274195</v>
@@ -8941,7 +8941,7 @@
         <v>0.9943510137388091</v>
       </c>
       <c r="C109" t="n">
-        <v>0.004575055152978852</v>
+        <v>0.005018471336220889</v>
       </c>
       <c r="D109" t="n">
         <v>-0.5970863784477247</v>
@@ -8956,7 +8956,7 @@
         <v>115.447</v>
       </c>
       <c r="H109" t="n">
-        <v>0.023089376</v>
+        <v>0.240573262856546</v>
       </c>
       <c r="I109" t="n">
         <v>-0.5970863784477247</v>
@@ -8975,7 +8975,7 @@
         <v>0.9946522119315668</v>
       </c>
       <c r="C110" t="n">
-        <v>0.005509655595497407</v>
+        <v>0.006071175449762156</v>
       </c>
       <c r="D110" t="n">
         <v>-0.5965079763688514</v>
@@ -8990,7 +8990,7 @@
         <v>115.351</v>
       </c>
       <c r="H110" t="n">
-        <v>0.023070229</v>
+        <v>0.296633355633458</v>
       </c>
       <c r="I110" t="n">
         <v>-0.5965079763688514</v>
@@ -9009,7 +9009,7 @@
         <v>0.993640572754817</v>
       </c>
       <c r="C111" t="n">
-        <v>0.001887100421278943</v>
+        <v>0.002430881362845545</v>
       </c>
       <c r="D111" t="n">
         <v>-0.5981342549897857</v>
@@ -9024,7 +9024,7 @@
         <v>115.138</v>
       </c>
       <c r="H111" t="n">
-        <v>0.023027636</v>
+        <v>0.179045623390476</v>
       </c>
       <c r="I111" t="n">
         <v>-0.5981342549897857</v>
@@ -9043,7 +9043,7 @@
         <v>0.977132219697786</v>
       </c>
       <c r="C112" t="n">
-        <v>0.003255716620761533</v>
+        <v>0.004816040650964057</v>
       </c>
       <c r="D112" t="n">
         <v>-0.7596292363509924</v>
@@ -9058,7 +9058,7 @@
         <v>119.647</v>
       </c>
       <c r="H112" t="n">
-        <v>0.023929451</v>
+        <v>0.435208535945917</v>
       </c>
       <c r="I112" t="n">
         <v>-0.7596292363509924</v>
@@ -9077,7 +9077,7 @@
         <v>0.9773777377782764</v>
       </c>
       <c r="C113" t="n">
-        <v>0.002509077375338799</v>
+        <v>0.003214420764724714</v>
       </c>
       <c r="D113" t="n">
         <v>-0.7592754993932411</v>
@@ -9092,7 +9092,7 @@
         <v>119.4</v>
       </c>
       <c r="H113" t="n">
-        <v>0.023879923</v>
+        <v>0.246614488138743</v>
       </c>
       <c r="I113" t="n">
         <v>-0.7592754993932411</v>
@@ -9111,7 +9111,7 @@
         <v>0.9774698177707487</v>
       </c>
       <c r="C114" t="n">
-        <v>0.002591407432822546</v>
+        <v>0.003486665134126356</v>
       </c>
       <c r="D114" t="n">
         <v>-0.7590793233862385</v>
@@ -9126,7 +9126,7 @@
         <v>119.415</v>
       </c>
       <c r="H114" t="n">
-        <v>0.023883058</v>
+        <v>0.285977791035725</v>
       </c>
       <c r="I114" t="n">
         <v>-0.7590793233862385</v>
@@ -9145,7 +9145,7 @@
         <v>0.976880099216017</v>
       </c>
       <c r="C115" t="n">
-        <v>0.001967682073466924</v>
+        <v>0.002964441127782051</v>
       </c>
       <c r="D115" t="n">
         <v>-0.7597501588892772</v>
@@ -9160,7 +9160,7 @@
         <v>119.144</v>
       </c>
       <c r="H115" t="n">
-        <v>0.023828851</v>
+        <v>0.27147042383661</v>
       </c>
       <c r="I115" t="n">
         <v>-0.7597501588892772</v>
@@ -9179,7 +9179,7 @@
         <v>0.9771757691242559</v>
       </c>
       <c r="C116" t="n">
-        <v>0.001595278247850214</v>
+        <v>0.002059321184343212</v>
       </c>
       <c r="D116" t="n">
         <v>-0.759467197854363</v>
@@ -9194,7 +9194,7 @@
         <v>119.028</v>
       </c>
       <c r="H116" t="n">
-        <v>0.023805565</v>
+        <v>0.160402725319686</v>
       </c>
       <c r="I116" t="n">
         <v>-0.759467197854363</v>
@@ -9213,7 +9213,7 @@
         <v>0.977264325783747</v>
       </c>
       <c r="C117" t="n">
-        <v>0.002108831940075859</v>
+        <v>0.003012596596071532</v>
       </c>
       <c r="D117" t="n">
         <v>-0.7592925282587082</v>
@@ -9228,7 +9228,7 @@
         <v>119.127</v>
       </c>
       <c r="H117" t="n">
-        <v>0.023825362</v>
+        <v>0.26333358753241</v>
       </c>
       <c r="I117" t="n">
         <v>-0.7592925282587082</v>
@@ -9247,7 +9247,7 @@
         <v>0.9776792250672337</v>
       </c>
       <c r="C118" t="n">
-        <v>0.003210387415244089</v>
+        <v>0.003956546042873001</v>
       </c>
       <c r="D118" t="n">
         <v>-0.7588672876817322</v>
@@ -9262,7 +9262,7 @@
         <v>118.982</v>
       </c>
       <c r="H118" t="n">
-        <v>0.023796364</v>
+        <v>0.282432166343944</v>
       </c>
       <c r="I118" t="n">
         <v>-0.7588672876817322</v>
@@ -9281,7 +9281,7 @@
         <v>0.9770412320295218</v>
       </c>
       <c r="C119" t="n">
-        <v>0.002123584633633482</v>
+        <v>0.00324355411289518</v>
       </c>
       <c r="D119" t="n">
         <v>-0.7595893450976803</v>
@@ -9296,7 +9296,7 @@
         <v>118.99</v>
       </c>
       <c r="H119" t="n">
-        <v>0.023798007</v>
+        <v>0.299534684511971</v>
       </c>
       <c r="I119" t="n">
         <v>-0.7595893450976803</v>
@@ -9315,7 +9315,7 @@
         <v>0.9772793926524992</v>
       </c>
       <c r="C120" t="n">
-        <v>0.002298462385526022</v>
+        <v>0.003019587663648546</v>
       </c>
       <c r="D120" t="n">
         <v>-0.75940482596714</v>
@@ -9330,7 +9330,7 @@
         <v>119.12</v>
       </c>
       <c r="H120" t="n">
-        <v>0.023823957</v>
+        <v>0.239883271123385</v>
       </c>
       <c r="I120" t="n">
         <v>-0.75940482596714</v>
@@ -9349,7 +9349,7 @@
         <v>0.976496140086431</v>
       </c>
       <c r="C121" t="n">
-        <v>0.002855034786768541</v>
+        <v>0.004251960801588668</v>
       </c>
       <c r="D121" t="n">
         <v>-0.7602017360284696</v>
@@ -9364,7 +9364,7 @@
         <v>119.119</v>
       </c>
       <c r="H121" t="n">
-        <v>0.023823831</v>
+        <v>0.385099439600387</v>
       </c>
       <c r="I121" t="n">
         <v>-0.7602017360284696</v>
@@ -9383,7 +9383,7 @@
         <v>0.9541296511929237</v>
       </c>
       <c r="C122" t="n">
-        <v>0.00352052019405556</v>
+        <v>0.004548043286417236</v>
       </c>
       <c r="D122" t="n">
         <v>-0.9489298025605883</v>
@@ -9398,7 +9398,7 @@
         <v>122.844</v>
       </c>
       <c r="H122" t="n">
-        <v>0.024568704</v>
+        <v>0.371528497544312</v>
       </c>
       <c r="I122" t="n">
         <v>-0.9489298025605883</v>
@@ -9417,7 +9417,7 @@
         <v>0.9537091168123721</v>
       </c>
       <c r="C123" t="n">
-        <v>0.002488703321096372</v>
+        <v>0.00359897232634437</v>
       </c>
       <c r="D123" t="n">
         <v>-0.9492894734206061</v>
@@ -9432,7 +9432,7 @@
         <v>122.676</v>
       </c>
       <c r="H123" t="n">
-        <v>0.024535121</v>
+        <v>0.335312127870267</v>
       </c>
       <c r="I123" t="n">
         <v>-0.9492894734206061</v>
@@ -9451,7 +9451,7 @@
         <v>0.9534665326893835</v>
       </c>
       <c r="C124" t="n">
-        <v>0.001834993207715379</v>
+        <v>0.002999313578757734</v>
       </c>
       <c r="D124" t="n">
         <v>-0.9495101185182167</v>
@@ -9466,7 +9466,7 @@
         <v>122.769</v>
       </c>
       <c r="H124" t="n">
-        <v>0.024553701</v>
+        <v>0.306467881685236</v>
       </c>
       <c r="I124" t="n">
         <v>-0.9495101185182167</v>
@@ -9485,7 +9485,7 @@
         <v>0.9537250651154463</v>
       </c>
       <c r="C125" t="n">
-        <v>0.002299525926997527</v>
+        <v>0.003019332865974025</v>
       </c>
       <c r="D125" t="n">
         <v>-0.9492472185373213</v>
@@ -9500,7 +9500,7 @@
         <v>122.777</v>
       </c>
       <c r="H125" t="n">
-        <v>0.024555325</v>
+        <v>0.253084129799715</v>
       </c>
       <c r="I125" t="n">
         <v>-0.9492472185373213</v>
@@ -9519,7 +9519,7 @@
         <v>0.9530257886449571</v>
       </c>
       <c r="C126" t="n">
-        <v>0.003873407886520117</v>
+        <v>0.005579207597709281</v>
       </c>
       <c r="D126" t="n">
         <v>-0.9498801016630445</v>
@@ -9534,7 +9534,7 @@
         <v>122.848</v>
       </c>
       <c r="H126" t="n">
-        <v>0.024569623</v>
+        <v>0.518193745559417</v>
       </c>
       <c r="I126" t="n">
         <v>-0.9498801016630445</v>
@@ -9553,7 +9553,7 @@
         <v>0.9532664419925558</v>
       </c>
       <c r="C127" t="n">
-        <v>0.001893271932260457</v>
+        <v>0.002633799189122271</v>
       </c>
       <c r="D127" t="n">
         <v>-0.9496571179323254</v>
@@ -9568,7 +9568,7 @@
         <v>122.94</v>
       </c>
       <c r="H127" t="n">
-        <v>0.024587957</v>
+        <v>0.237410449174721</v>
       </c>
       <c r="I127" t="n">
         <v>-0.9496571179323254</v>
@@ -9587,7 +9587,7 @@
         <v>0.9539330808202905</v>
       </c>
       <c r="C128" t="n">
-        <v>0.002945578975113296</v>
+        <v>0.004234726656692727</v>
       </c>
       <c r="D128" t="n">
         <v>-0.9491564302578315</v>
@@ -9602,7 +9602,7 @@
         <v>123.387</v>
       </c>
       <c r="H128" t="n">
-        <v>0.024677443</v>
+        <v>0.394299766723677</v>
       </c>
       <c r="I128" t="n">
         <v>-0.9491564302578315</v>
@@ -9621,7 +9621,7 @@
         <v>0.9531039332102981</v>
       </c>
       <c r="C129" t="n">
-        <v>0.001790550129442137</v>
+        <v>0.002589587194945757</v>
       </c>
       <c r="D129" t="n">
         <v>-0.9498168403947123</v>
@@ -9636,7 +9636,7 @@
         <v>122.966</v>
       </c>
       <c r="H129" t="n">
-        <v>0.024593212</v>
+        <v>0.242613485792308</v>
       </c>
       <c r="I129" t="n">
         <v>-0.9498168403947123</v>
@@ -9655,7 +9655,7 @@
         <v>0.9538901949936344</v>
       </c>
       <c r="C130" t="n">
-        <v>0.002585285132760562</v>
+        <v>0.003468745439540308</v>
       </c>
       <c r="D130" t="n">
         <v>-0.9491429471997908</v>
@@ -9670,7 +9670,7 @@
         <v>122.736</v>
       </c>
       <c r="H130" t="n">
-        <v>0.024547108</v>
+        <v>0.298580930458355</v>
       </c>
       <c r="I130" t="n">
         <v>-0.9491429471997908</v>
@@ -9689,7 +9689,7 @@
         <v>0.952835204003287</v>
       </c>
       <c r="C131" t="n">
-        <v>0.003873431596101744</v>
+        <v>0.00506478877843171</v>
       </c>
       <c r="D131" t="n">
         <v>-0.9500188749385403</v>
@@ -9704,7 +9704,7 @@
         <v>123.39</v>
       </c>
       <c r="H131" t="n">
-        <v>0.024677904</v>
+        <v>0.423299719857778</v>
       </c>
       <c r="I131" t="n">
         <v>-0.9500188749385403</v>
@@ -9723,7 +9723,7 @@
         <v>0.9165779630276262</v>
       </c>
       <c r="C132" t="n">
-        <v>0.002758622988913007</v>
+        <v>0.003332264510477786</v>
       </c>
       <c r="D132" t="n">
         <v>-1.186580235218716</v>
@@ -9738,7 +9738,7 @@
         <v>124.849</v>
       </c>
       <c r="H132" t="n">
-        <v>0.024969882</v>
+        <v>0.255831935996893</v>
       </c>
       <c r="I132" t="n">
         <v>-1.186580235218716</v>
@@ -9757,7 +9757,7 @@
         <v>0.9161927095137331</v>
       </c>
       <c r="C133" t="n">
-        <v>0.002082840461689428</v>
+        <v>0.002937335903084928</v>
       </c>
       <c r="D133" t="n">
         <v>-1.186931408591655</v>
@@ -9772,7 +9772,7 @@
         <v>125.565</v>
       </c>
       <c r="H133" t="n">
-        <v>0.025113098</v>
+        <v>0.284963460948001</v>
       </c>
       <c r="I133" t="n">
         <v>-1.186931408591655</v>
@@ -9791,7 +9791,7 @@
         <v>0.9164746491661087</v>
       </c>
       <c r="C134" t="n">
-        <v>0.002620327193440102</v>
+        <v>0.003779180210274635</v>
       </c>
       <c r="D134" t="n">
         <v>-1.186624936693005</v>
@@ -9806,7 +9806,7 @@
         <v>125.114</v>
       </c>
       <c r="H134" t="n">
-        <v>0.025022711</v>
+        <v>0.372609921687144</v>
       </c>
       <c r="I134" t="n">
         <v>-1.186624936693005</v>
@@ -9825,7 +9825,7 @@
         <v>0.9156005847838052</v>
       </c>
       <c r="C135" t="n">
-        <v>0.004317784767575751</v>
+        <v>0.00629216162102221</v>
       </c>
       <c r="D135" t="n">
         <v>-1.187158541512341</v>
@@ -9840,7 +9840,7 @@
         <v>124.745</v>
       </c>
       <c r="H135" t="n">
-        <v>0.024949005</v>
+        <v>0.624073916115064</v>
       </c>
       <c r="I135" t="n">
         <v>-1.187158541512341</v>
@@ -9859,7 +9859,7 @@
         <v>0.9161802403790318</v>
       </c>
       <c r="C136" t="n">
-        <v>0.0007967290817473758</v>
+        <v>0.001078019844408058</v>
       </c>
       <c r="D136" t="n">
         <v>-1.186774132225347</v>
@@ -9874,7 +9874,7 @@
         <v>124.705</v>
       </c>
       <c r="H136" t="n">
-        <v>0.024941045</v>
+        <v>0.101942526494804</v>
       </c>
       <c r="I136" t="n">
         <v>-1.186774132225347</v>
@@ -9893,7 +9893,7 @@
         <v>0.9161709685855326</v>
       </c>
       <c r="C137" t="n">
-        <v>0.001623788431388811</v>
+        <v>0.002261973186875156</v>
       </c>
       <c r="D137" t="n">
         <v>-1.186820647904797</v>
@@ -9908,7 +9908,7 @@
         <v>124.719</v>
       </c>
       <c r="H137" t="n">
-        <v>0.024943833</v>
+        <v>0.215817993275089</v>
       </c>
       <c r="I137" t="n">
         <v>-1.186820647904797</v>
@@ -9927,7 +9927,7 @@
         <v>0.9163709886390076</v>
       </c>
       <c r="C138" t="n">
-        <v>0.001271456553351721</v>
+        <v>0.001858252007213771</v>
       </c>
       <c r="D138" t="n">
         <v>-1.186710365962002</v>
@@ -9942,7 +9942,7 @@
         <v>124.848</v>
       </c>
       <c r="H138" t="n">
-        <v>0.024969691</v>
+        <v>0.186312215408515</v>
       </c>
       <c r="I138" t="n">
         <v>-1.186710365962002</v>
@@ -9961,7 +9961,7 @@
         <v>0.9162484054918366</v>
       </c>
       <c r="C139" t="n">
-        <v>0.002580845846603492</v>
+        <v>0.003463416466368283</v>
       </c>
       <c r="D139" t="n">
         <v>-1.186780988970187</v>
@@ -9976,7 +9976,7 @@
         <v>125.483</v>
       </c>
       <c r="H139" t="n">
-        <v>0.025096507</v>
+        <v>0.317307755504802</v>
       </c>
       <c r="I139" t="n">
         <v>-1.186780988970187</v>
@@ -9995,7 +9995,7 @@
         <v>0.916333622678056</v>
       </c>
       <c r="C140" t="n">
-        <v>0.00157308392351989</v>
+        <v>0.002215986416729693</v>
       </c>
       <c r="D140" t="n">
         <v>-1.186701620199536</v>
@@ -10010,7 +10010,7 @@
         <v>124.811</v>
       </c>
       <c r="H140" t="n">
-        <v>0.02496217</v>
+        <v>0.214048217231555</v>
       </c>
       <c r="I140" t="n">
         <v>-1.186701620199536</v>
@@ -10029,7 +10029,7 @@
         <v>0.9161959483144212</v>
       </c>
       <c r="C141" t="n">
-        <v>0.003392895574455821</v>
+        <v>0.004993590101270004</v>
       </c>
       <c r="D141" t="n">
         <v>-1.186773062639309</v>
@@ -10044,7 +10044,7 @@
         <v>124.888</v>
       </c>
       <c r="H141" t="n">
-        <v>0.02497762</v>
+        <v>0.500056445885356</v>
       </c>
       <c r="I141" t="n">
         <v>-1.186773062639309</v>
@@ -10063,7 +10063,7 @@
         <v>0.8537166402900869</v>
       </c>
       <c r="C142" t="n">
-        <v>0.002196010453649702</v>
+        <v>0.003446057772278755</v>
       </c>
       <c r="D142" t="n">
         <v>-1.518937567689745</v>
@@ -10078,7 +10078,7 @@
         <v>126.716</v>
       </c>
       <c r="H142" t="n">
-        <v>0.025343238</v>
+        <v>0.394998860209947</v>
       </c>
       <c r="I142" t="n">
         <v>-1.518937567689745</v>
@@ -10097,7 +10097,7 @@
         <v>0.8539019817307391</v>
       </c>
       <c r="C143" t="n">
-        <v>0.001534511180430807</v>
+        <v>0.002257198237017802</v>
       </c>
       <c r="D143" t="n">
         <v>-1.518823543825993</v>
@@ -10112,7 +10112,7 @@
         <v>126.52</v>
       </c>
       <c r="H143" t="n">
-        <v>0.025304013</v>
+        <v>0.246571485972701</v>
       </c>
       <c r="I143" t="n">
         <v>-1.518823543825993</v>
@@ -10131,7 +10131,7 @@
         <v>0.8537275993475835</v>
       </c>
       <c r="C144" t="n">
-        <v>0.001628807617440066</v>
+        <v>0.002284561191862455</v>
       </c>
       <c r="D144" t="n">
         <v>-1.518931350802526</v>
@@ -10146,7 +10146,7 @@
         <v>126.848</v>
       </c>
       <c r="H144" t="n">
-        <v>0.025369601</v>
+        <v>0.239366337199363</v>
       </c>
       <c r="I144" t="n">
         <v>-1.518931350802526</v>
@@ -10165,7 +10165,7 @@
         <v>0.8540196889231098</v>
       </c>
       <c r="C145" t="n">
-        <v>0.001512282544325826</v>
+        <v>0.0019802064760506</v>
       </c>
       <c r="D145" t="n">
         <v>-1.518758754548577</v>
@@ -10180,7 +10180,7 @@
         <v>127.202</v>
       </c>
       <c r="H145" t="n">
-        <v>0.02544031</v>
+        <v>0.192098285068366</v>
       </c>
       <c r="I145" t="n">
         <v>-1.518758754548577</v>
@@ -10199,7 +10199,7 @@
         <v>0.8538386783932411</v>
       </c>
       <c r="C146" t="n">
-        <v>0.001255851242978765</v>
+        <v>0.001718364193307598</v>
       </c>
       <c r="D146" t="n">
         <v>-1.518838544036293</v>
@@ -10214,7 +10214,7 @@
         <v>126.625</v>
       </c>
       <c r="H146" t="n">
-        <v>0.025324908</v>
+        <v>0.17577088995927</v>
       </c>
       <c r="I146" t="n">
         <v>-1.518838544036293</v>
@@ -10233,7 +10233,7 @@
         <v>0.8539045660047971</v>
       </c>
       <c r="C147" t="n">
-        <v>0.00162656558085253</v>
+        <v>0.002531695193224192</v>
       </c>
       <c r="D147" t="n">
         <v>-1.518819918207938</v>
@@ -10248,7 +10248,7 @@
         <v>126.754</v>
       </c>
       <c r="H147" t="n">
-        <v>0.025350843</v>
+        <v>0.28909449313744</v>
       </c>
       <c r="I147" t="n">
         <v>-1.518819918207938</v>
@@ -10267,7 +10267,7 @@
         <v>0.853751444335992</v>
       </c>
       <c r="C148" t="n">
-        <v>0.002112925860926384</v>
+        <v>0.003030265346808853</v>
       </c>
       <c r="D148" t="n">
         <v>-1.518925884532245</v>
@@ -10282,7 +10282,7 @@
         <v>127.033</v>
       </c>
       <c r="H148" t="n">
-        <v>0.025406507</v>
+        <v>0.324193442090004</v>
       </c>
       <c r="I148" t="n">
         <v>-1.518925884532245</v>
@@ -10301,7 +10301,7 @@
         <v>0.8534848452334569</v>
       </c>
       <c r="C149" t="n">
-        <v>0.002295354905862594</v>
+        <v>0.003309736205381312</v>
       </c>
       <c r="D149" t="n">
         <v>-1.519087181449516</v>
@@ -10316,7 +10316,7 @@
         <v>126.622</v>
       </c>
       <c r="H149" t="n">
-        <v>0.025324415</v>
+        <v>0.354662509289587</v>
       </c>
       <c r="I149" t="n">
         <v>-1.519087181449516</v>
@@ -10335,7 +10335,7 @@
         <v>0.8540664710598472</v>
       </c>
       <c r="C150" t="n">
-        <v>0.001542759105635947</v>
+        <v>0.002056983411368044</v>
       </c>
       <c r="D150" t="n">
         <v>-1.518727038605024</v>
@@ -10350,7 +10350,7 @@
         <v>126.517</v>
       </c>
       <c r="H150" t="n">
-        <v>0.025303425</v>
+        <v>0.20312588992399</v>
       </c>
       <c r="I150" t="n">
         <v>-1.518727038605024</v>
@@ -10369,7 +10369,7 @@
         <v>0.8538077921184046</v>
       </c>
       <c r="C151" t="n">
-        <v>0.002393332709695696</v>
+        <v>0.003583659908347265</v>
       </c>
       <c r="D151" t="n">
         <v>-1.518904461856806</v>
@@ -10384,7 +10384,7 @@
         <v>126.726</v>
       </c>
       <c r="H151" t="n">
-        <v>0.025345273</v>
+        <v>0.396705597323135</v>
       </c>
       <c r="I151" t="n">
         <v>-1.518904461856806</v>
@@ -10403,7 +10403,7 @@
         <v>0.7682038651522488</v>
       </c>
       <c r="C152" t="n">
-        <v>0.001786309723362741</v>
+        <v>0.002290703078664681</v>
       </c>
       <c r="D152" t="n">
         <v>-1.898589827761933</v>
@@ -10418,7 +10418,7 @@
         <v>126.591</v>
       </c>
       <c r="H152" t="n">
-        <v>0.025318225</v>
+        <v>0.237662403228966</v>
       </c>
       <c r="I152" t="n">
         <v>-1.898589827761933</v>
@@ -10437,7 +10437,7 @@
         <v>0.7674482686022198</v>
       </c>
       <c r="C153" t="n">
-        <v>0.002409760303162789</v>
+        <v>0.003505335079692655</v>
       </c>
       <c r="D153" t="n">
         <v>-1.899042664673275</v>
@@ -10452,7 +10452,7 @@
         <v>126.722</v>
       </c>
       <c r="H153" t="n">
-        <v>0.025344364</v>
+        <v>0.421107313409021</v>
       </c>
       <c r="I153" t="n">
         <v>-1.899042664673275</v>
@@ -10471,7 +10471,7 @@
         <v>0.7677683733378668</v>
       </c>
       <c r="C154" t="n">
-        <v>0.001494454718159408</v>
+        <v>0.002418982693815641</v>
       </c>
       <c r="D154" t="n">
         <v>-1.898864387823961</v>
@@ -10486,7 +10486,7 @@
         <v>126.703</v>
       </c>
       <c r="H154" t="n">
-        <v>0.025340616</v>
+        <v>0.314924497437384</v>
       </c>
       <c r="I154" t="n">
         <v>-1.898864387823961</v>
@@ -10505,7 +10505,7 @@
         <v>0.7677624394224872</v>
       </c>
       <c r="C155" t="n">
-        <v>0.0009110532213234339</v>
+        <v>0.001410843045374895</v>
       </c>
       <c r="D155" t="n">
         <v>-1.898836092833925</v>
@@ -10520,7 +10520,7 @@
         <v>126.179</v>
       </c>
       <c r="H155" t="n">
-        <v>0.025235848</v>
+        <v>0.178831140683067</v>
       </c>
       <c r="I155" t="n">
         <v>-1.898836092833925</v>
@@ -10539,7 +10539,7 @@
         <v>0.7672834720240541</v>
       </c>
       <c r="C156" t="n">
-        <v>0.00296731269902812</v>
+        <v>0.004057882353452721</v>
       </c>
       <c r="D156" t="n">
         <v>-1.89914176301677</v>
@@ -10554,7 +10554,7 @@
         <v>126.634</v>
       </c>
       <c r="H156" t="n">
-        <v>0.02532687</v>
+        <v>0.45752707883284</v>
       </c>
       <c r="I156" t="n">
         <v>-1.89914176301677</v>
@@ -10573,7 +10573,7 @@
         <v>0.7675176941755193</v>
       </c>
       <c r="C157" t="n">
-        <v>0.001992928059122261</v>
+        <v>0.002567165576306638</v>
       </c>
       <c r="D157" t="n">
         <v>-1.899003934365898</v>
@@ -10588,7 +10588,7 @@
         <v>127.047</v>
       </c>
       <c r="H157" t="n">
-        <v>0.025409471</v>
+        <v>0.269062985584301</v>
       </c>
       <c r="I157" t="n">
         <v>-1.899003934365898</v>
@@ -10607,7 +10607,7 @@
         <v>0.7678182702325892</v>
       </c>
       <c r="C158" t="n">
-        <v>0.0008601235613632995</v>
+        <v>0.001175411444443341</v>
       </c>
       <c r="D158" t="n">
         <v>-1.898816833625994</v>
@@ -10622,7 +10622,7 @@
         <v>126.347</v>
       </c>
       <c r="H158" t="n">
-        <v>0.025269313</v>
+        <v>0.134225556778271</v>
       </c>
       <c r="I158" t="n">
         <v>-1.898816833625994</v>
@@ -10641,7 +10641,7 @@
         <v>0.7673586675447344</v>
       </c>
       <c r="C159" t="n">
-        <v>0.001952833231211985</v>
+        <v>0.00237073113573666</v>
       </c>
       <c r="D159" t="n">
         <v>-1.899057307546973</v>
@@ -10656,7 +10656,7 @@
         <v>126.345</v>
       </c>
       <c r="H159" t="n">
-        <v>0.025268999</v>
+        <v>0.222755358151639</v>
       </c>
       <c r="I159" t="n">
         <v>-1.899057307546973</v>
@@ -10675,7 +10675,7 @@
         <v>0.7674007994372982</v>
       </c>
       <c r="C160" t="n">
-        <v>0.002123758542342436</v>
+        <v>0.002740902713847036</v>
       </c>
       <c r="D160" t="n">
         <v>-1.899080665398786</v>
@@ -10690,7 +10690,7 @@
         <v>126.436</v>
       </c>
       <c r="H160" t="n">
-        <v>0.025287156</v>
+        <v>0.286592794241622</v>
       </c>
       <c r="I160" t="n">
         <v>-1.899080665398786</v>
@@ -10709,7 +10709,7 @@
         <v>0.76774626200166</v>
       </c>
       <c r="C161" t="n">
-        <v>0.001243945519867335</v>
+        <v>0.001870591969119206</v>
       </c>
       <c r="D161" t="n">
         <v>-1.898878061643849</v>
@@ -10724,7 +10724,7 @@
         <v>126.547</v>
       </c>
       <c r="H161" t="n">
-        <v>0.025309323</v>
+        <v>0.231659276413865</v>
       </c>
       <c r="I161" t="n">
         <v>-1.898878061643849</v>
@@ -10743,7 +10743,7 @@
         <v>0.643647877621464</v>
       </c>
       <c r="C162" t="n">
-        <v>0.001330767763937959</v>
+        <v>0.001697115123052046</v>
       </c>
       <c r="D162" t="n">
         <v>-2.373597696771729</v>
@@ -10758,7 +10758,7 @@
         <v>126.107</v>
       </c>
       <c r="H162" t="n">
-        <v>0.025221348</v>
+        <v>0.207886793909562</v>
       </c>
       <c r="I162" t="n">
         <v>-2.373597696771729</v>
@@ -10777,7 +10777,7 @@
         <v>0.644136441947274</v>
       </c>
       <c r="C163" t="n">
-        <v>0.001292722958397157</v>
+        <v>0.001624745426498554</v>
       </c>
       <c r="D163" t="n">
         <v>-2.37325950540645</v>
@@ -10792,7 +10792,7 @@
         <v>126.001</v>
       </c>
       <c r="H163" t="n">
-        <v>0.02520023</v>
+        <v>0.194165422532447</v>
       </c>
       <c r="I163" t="n">
         <v>-2.37325950540645</v>
@@ -10811,7 +10811,7 @@
         <v>0.644298778778711</v>
       </c>
       <c r="C164" t="n">
-        <v>0.002559571885455578</v>
+        <v>0.003358232957458336</v>
       </c>
       <c r="D164" t="n">
         <v>-2.373180416349297</v>
@@ -10826,7 +10826,7 @@
         <v>125.886</v>
       </c>
       <c r="H164" t="n">
-        <v>0.025177128</v>
+        <v>0.425513417690816</v>
       </c>
       <c r="I164" t="n">
         <v>-2.373180416349297</v>
@@ -10845,7 +10845,7 @@
         <v>0.6438666362961364</v>
       </c>
       <c r="C165" t="n">
-        <v>0.00174789059171001</v>
+        <v>0.002612594634655217</v>
       </c>
       <c r="D165" t="n">
         <v>-2.373449453611761</v>
@@ -10860,7 +10860,7 @@
         <v>125.958</v>
       </c>
       <c r="H165" t="n">
-        <v>0.025191638</v>
+        <v>0.380700896151338</v>
       </c>
       <c r="I165" t="n">
         <v>-2.373449453611761</v>
@@ -10879,7 +10879,7 @@
         <v>0.6439375518524958</v>
       </c>
       <c r="C166" t="n">
-        <v>0.001803478170396795</v>
+        <v>0.002789662966514157</v>
       </c>
       <c r="D166" t="n">
         <v>-2.373395375307986</v>
@@ -10894,7 +10894,7 @@
         <v>125.973</v>
       </c>
       <c r="H166" t="n">
-        <v>0.025194517</v>
+        <v>0.417120400719826</v>
       </c>
       <c r="I166" t="n">
         <v>-2.373395375307986</v>
@@ -10913,7 +10913,7 @@
         <v>0.6437934038996345</v>
       </c>
       <c r="C167" t="n">
-        <v>0.00114285237459502</v>
+        <v>0.001498620077091551</v>
       </c>
       <c r="D167" t="n">
         <v>-2.373483785676584</v>
@@ -10928,7 +10928,7 @@
         <v>126.246</v>
       </c>
       <c r="H167" t="n">
-        <v>0.025249135</v>
+        <v>0.191767424016524</v>
       </c>
       <c r="I167" t="n">
         <v>-2.373483785676584</v>
@@ -10947,7 +10947,7 @@
         <v>0.6438774804572911</v>
       </c>
       <c r="C168" t="n">
-        <v>0.001514294878484339</v>
+        <v>0.002294288891974608</v>
       </c>
       <c r="D168" t="n">
         <v>-2.373437763512482</v>
@@ -10962,7 +10962,7 @@
         <v>126.356</v>
       </c>
       <c r="H168" t="n">
-        <v>0.025271213</v>
+        <v>0.339178903187766</v>
       </c>
       <c r="I168" t="n">
         <v>-2.373437763512482</v>
@@ -10981,7 +10981,7 @@
         <v>0.6440538802373571</v>
       </c>
       <c r="C169" t="n">
-        <v>0.001722506386205171</v>
+        <v>0.002550174647580746</v>
       </c>
       <c r="D169" t="n">
         <v>-2.373321900953357</v>
@@ -10996,7 +10996,7 @@
         <v>126.635</v>
       </c>
       <c r="H169" t="n">
-        <v>0.025326942</v>
+        <v>0.370617894134587</v>
       </c>
       <c r="I169" t="n">
         <v>-2.373321900953357</v>
@@ -11015,7 +11015,7 @@
         <v>0.6439495957148142</v>
       </c>
       <c r="C170" t="n">
-        <v>0.001494460295682958</v>
+        <v>0.00203674961314073</v>
       </c>
       <c r="D170" t="n">
         <v>-2.373392370945519</v>
@@ -11030,7 +11030,7 @@
         <v>125.757</v>
       </c>
       <c r="H170" t="n">
-        <v>0.025151493</v>
+        <v>0.271412840631505</v>
       </c>
       <c r="I170" t="n">
         <v>-2.373392370945519</v>
@@ -11049,7 +11049,7 @@
         <v>0.6441385187123638</v>
       </c>
       <c r="C171" t="n">
-        <v>0.001360858696768395</v>
+        <v>0.001502169482784269</v>
       </c>
       <c r="D171" t="n">
         <v>-2.373280389812181</v>
@@ -11064,7 +11064,7 @@
         <v>125.81</v>
       </c>
       <c r="H171" t="n">
-        <v>0.025161996</v>
+        <v>0.126755357843512</v>
       </c>
       <c r="I171" t="n">
         <v>-2.373280389812181</v>

</xml_diff>

<commit_message>
Change labels but only for diagrams relevant to the paper. Others will be updates soon
</commit_message>
<xml_diff>
--- a/All_datasets.xlsx
+++ b/All_datasets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="CEM" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -5225,7 +5225,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -10561,6 +10561,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
delete np.abs in front of the phase difference in Case study_2.ipynb and add (\omega) to labels relevant to paper
</commit_message>
<xml_diff>
--- a/All_datasets.xlsx
+++ b/All_datasets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="CEM" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -5225,7 +5225,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -10561,6 +10561,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correct results for Case study 2 and Clean Introduction and Case study 2
</commit_message>
<xml_diff>
--- a/All_datasets.xlsx
+++ b/All_datasets.xlsx
@@ -437,42 +437,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Frequency [Hz]</t>
+          <t>Frequency in Hz</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>$x_{M},$ [m s^-2/m s^-2]</t>
+          <t>$|S(\omega)|$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>$U_{M},$ [m s^-2/m s^-2]</t>
+          <t>$U_{|S(\omega)|}$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>$x_{\phi},$ [rad]</t>
+          <t>$\varphi(\omega)$ in $rad$</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>$U_{\phi},$ [rad]</t>
+          <t>$U_{\varphi(\omega)}$ in $rad$</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Excitation_freq [Hz]</t>
+          <t>Excitation_freq in Hz</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>$x_{Aexcit},$ [m s^-2/m s^-2]</t>
+          <t>$A_{excit}$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>$U_{Aexcit},$ [m s^-2/m s^-2]</t>
+          <t>$U_{Aexcit}$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -5246,42 +5246,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Frequency [Hz]</t>
+          <t>Frequency in Hz</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>$x_{M},$ [m s^-2/m s^-2]</t>
+          <t>$|S(\omega)|$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>$U_{M},$ [m s^-2/m s^-2]</t>
+          <t>$U_{|S(\omega)|}$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>$x_{\phi},$ [rad]</t>
+          <t>$\varphi(\omega)$ in $rad$</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>$U_{\phi},$ [rad]</t>
+          <t>$U_{\varphi(\omega)}$ in $rad$</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Excitation_freq [Hz]</t>
+          <t>Excitation_freq in Hz</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>$x_{Aexcit},$ [m s^-2/m s^-2]</t>
+          <t>$A_{excit}$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>$U_{Aexcit},$ [m s^-2/m s^-2]</t>
+          <t>$U_{Aexcit}$ in $ \frac{\mathrm{m s}^-2}{\mathrm{m s}^-2}$</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">

</xml_diff>